<commit_message>
add updated tract names
</commit_message>
<xml_diff>
--- a/tracts/tract_names.xlsx
+++ b/tracts/tract_names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micheleclaibourn/Box Sync/mpc/dataForDemocracy/nsfcope/tracts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micheleclaibourn/Box Sync/mpc/dataForDemocracy/nsfcope/eastern_shore/tracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DBDCDB-B277-EF4F-ABF6-280E40D4270F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D49E3B-D39D-7A4F-84F1-90874FE514EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2760" windowWidth="27640" windowHeight="16940" xr2:uid="{1554B8D8-10F4-6B41-B1B3-EE727B9E603B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>locality</t>
   </si>
@@ -107,6 +107,51 @@
   </si>
   <si>
     <t>Marsh? (some people near western edge), Wallops Island</t>
+  </si>
+  <si>
+    <t>names_initial</t>
+  </si>
+  <si>
+    <t>Assateague</t>
+  </si>
+  <si>
+    <t>Horntown Area</t>
+  </si>
+  <si>
+    <t>Bullbegger Area, Oakhall</t>
+  </si>
+  <si>
+    <t>Bayside</t>
+  </si>
+  <si>
+    <t>Onancock</t>
+  </si>
+  <si>
+    <t>Pungoteague Area, South Accomack Bayside</t>
+  </si>
+  <si>
+    <t>Exmore Area</t>
+  </si>
+  <si>
+    <t>Machipongo, Nassawadox/Eastville Area</t>
+  </si>
+  <si>
+    <t>Cape Charles</t>
+  </si>
+  <si>
+    <t>Lower Northamponton, County Seaside</t>
+  </si>
+  <si>
+    <t>Wachapreague Area, South Accomack Seaside</t>
+  </si>
+  <si>
+    <t>Accomac</t>
+  </si>
+  <si>
+    <t>Nelsonia/Gargatha Area</t>
+  </si>
+  <si>
+    <t>Wallops Island Area</t>
   </si>
 </sst>
 </file>
@@ -467,18 +512,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C80D05FB-3A7E-E143-A4EB-26B830C4220D}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="26.5" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -491,8 +538,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>14</v>
       </c>
@@ -502,11 +552,14 @@
       <c r="C2" s="1">
         <v>90300</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>13</v>
       </c>
@@ -519,8 +572,11 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -530,11 +586,14 @@
       <c r="C4" s="2">
         <v>90600</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>11</v>
       </c>
@@ -544,11 +603,14 @@
       <c r="C5" s="2">
         <v>90700</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>10</v>
       </c>
@@ -558,11 +620,14 @@
       <c r="C6" s="2">
         <v>90800</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>9</v>
       </c>
@@ -572,11 +637,14 @@
       <c r="C7" s="2">
         <v>90402</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -586,11 +654,14 @@
       <c r="C8" s="2">
         <v>90401</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -600,11 +671,14 @@
       <c r="C9" s="2">
         <v>980200</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -614,11 +688,11 @@
       <c r="C10" s="2">
         <v>90102</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -628,11 +702,14 @@
       <c r="C11" s="2">
         <v>90101</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -642,11 +719,14 @@
       <c r="C12" s="2">
         <v>980100</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -656,11 +736,14 @@
       <c r="C13" s="2">
         <v>90201</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -670,11 +753,14 @@
       <c r="C14" s="2">
         <v>90202</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -684,11 +770,11 @@
       <c r="C15" s="2">
         <v>990100</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>4</v>
       </c>
@@ -698,11 +784,14 @@
       <c r="C16" s="2">
         <v>930301</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -712,11 +801,14 @@
       <c r="C17" s="2">
         <v>930302</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -726,11 +818,14 @@
       <c r="C18" s="1">
         <v>930100</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -740,39 +835,42 @@
       <c r="C19" s="1">
         <v>930200</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="2"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>